<commit_message>
fixed formatting in excel
</commit_message>
<xml_diff>
--- a/camera_snow_estimate_timeline.xlsx
+++ b/camera_snow_estimate_timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1803229\Documents\Snowstradamus\Snowstradamus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7A4A96-6857-42F2-A36A-0BF2B9B444A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E554CD99-1562-4EA0-8CC7-A37C6843E884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11292" yWindow="2004" windowWidth="17280" windowHeight="10044" xr2:uid="{C4BA0D95-1C30-456C-B2BA-46850E4E26C1}"/>
+    <workbookView xWindow="5760" yWindow="2004" windowWidth="17280" windowHeight="10044" xr2:uid="{C4BA0D95-1C30-456C-B2BA-46850E4E26C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,6 +70,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -101,7 +104,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,14 +421,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0BDC52-0678-4879-BFA4-045E88D6C76C}">
   <dimension ref="A1:D682"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A646" workbookViewId="0">
-      <selection activeCell="F668" sqref="F668"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -9982,5 +9985,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>